<commit_message>
stm32 more changes and bug fixes
-STM32 startup code now in C (using minimalistic driver)
-fixed bug in pin configuration macro
-removed tinyusb hal for testing
</commit_message>
<xml_diff>
--- a/docs/stm32f1_mcumap_gen.xlsx
+++ b/docs/stm32f1_mcumap_gen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCEM\Documents\GitHub\uCNC\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AFCE7B-5A10-4E63-8916-2AF48D8A2359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92930652-39AB-4697-B829-CA426C44322C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56:F69"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -870,7 +870,7 @@
 #define "&amp;C3&amp;"_CROFF "&amp;C3&amp;"_BIT
 #define "&amp;C3&amp;"_CR CRL
 #else
-#define "&amp;C3&amp;"_CROFF ("&amp;C3&amp;"_BIT&amp;0x03)
+#define "&amp;C3&amp;"_CROFF ("&amp;C3&amp;"_BIT&amp;0x05)
 #define "&amp;C3&amp;"_CR CRH
 #endif
 #define "&amp;B3&amp;" "&amp;A3&amp;"
@@ -889,7 +889,7 @@
 #define STEP0_CROFF STEP0_BIT
 #define STEP0_CR CRL
 #else
-#define STEP0_CROFF (STEP0_BIT&amp;0x03)
+#define STEP0_CROFF (STEP0_BIT&amp;0x05)
 #define STEP0_CR CRH
 #endif
 #define DIO0 0
@@ -990,7 +990,7 @@
 #define "&amp;C4&amp;"_CROFF "&amp;C4&amp;"_BIT
 #define "&amp;C4&amp;"_CR CRL
 #else
-#define "&amp;C4&amp;"_CROFF ("&amp;C4&amp;"_BIT&amp;0x03)
+#define "&amp;C4&amp;"_CROFF ("&amp;C4&amp;"_BIT&amp;0x05)
 #define "&amp;C4&amp;"_CR CRH
 #endif
 #define "&amp;B4&amp;" "&amp;A4&amp;"
@@ -1009,7 +1009,7 @@
 #define STEP1_CROFF STEP1_BIT
 #define STEP1_CR CRL
 #else
-#define STEP1_CROFF (STEP1_BIT&amp;0x03)
+#define STEP1_CROFF (STEP1_BIT&amp;0x05)
 #define STEP1_CR CRH
 #endif
 #define DIO1 1
@@ -1111,7 +1111,7 @@
 #define STEP2_CROFF STEP2_BIT
 #define STEP2_CR CRL
 #else
-#define STEP2_CROFF (STEP2_BIT&amp;0x03)
+#define STEP2_CROFF (STEP2_BIT&amp;0x05)
 #define STEP2_CR CRH
 #endif
 #define DIO2 2
@@ -1198,7 +1198,7 @@
 #define STEP3_CROFF STEP3_BIT
 #define STEP3_CR CRL
 #else
-#define STEP3_CROFF (STEP3_BIT&amp;0x03)
+#define STEP3_CROFF (STEP3_BIT&amp;0x05)
 #define STEP3_CR CRH
 #endif
 #define DIO3 3
@@ -1285,7 +1285,7 @@
 #define STEP4_CROFF STEP4_BIT
 #define STEP4_CR CRL
 #else
-#define STEP4_CROFF (STEP4_BIT&amp;0x03)
+#define STEP4_CROFF (STEP4_BIT&amp;0x05)
 #define STEP4_CR CRH
 #endif
 #define DIO4 4
@@ -1372,7 +1372,7 @@
 #define STEP5_CROFF STEP5_BIT
 #define STEP5_CR CRL
 #else
-#define STEP5_CROFF (STEP5_BIT&amp;0x03)
+#define STEP5_CROFF (STEP5_BIT&amp;0x05)
 #define STEP5_CR CRH
 #endif
 #define DIO5 5
@@ -1459,7 +1459,7 @@
 #define STEP6_CROFF STEP6_BIT
 #define STEP6_CR CRL
 #else
-#define STEP6_CROFF (STEP6_BIT&amp;0x03)
+#define STEP6_CROFF (STEP6_BIT&amp;0x05)
 #define STEP6_CR CRH
 #endif
 #define DIO6 6
@@ -1524,7 +1524,7 @@
 #define STEP7_CROFF STEP7_BIT
 #define STEP7_CR CRL
 #else
-#define STEP7_CROFF (STEP7_BIT&amp;0x03)
+#define STEP7_CROFF (STEP7_BIT&amp;0x05)
 #define STEP7_CR CRH
 #endif
 #define DIO7 7
@@ -1589,7 +1589,7 @@
 #define STEP0_EN_CROFF STEP0_EN_BIT
 #define STEP0_EN_CR CRL
 #else
-#define STEP0_EN_CROFF (STEP0_EN_BIT&amp;0x03)
+#define STEP0_EN_CROFF (STEP0_EN_BIT&amp;0x05)
 #define STEP0_EN_CR CRH
 #endif
 #define DIO8 8
@@ -1676,7 +1676,7 @@
 #define STEP1_EN_CROFF STEP1_EN_BIT
 #define STEP1_EN_CR CRL
 #else
-#define STEP1_EN_CROFF (STEP1_EN_BIT&amp;0x03)
+#define STEP1_EN_CROFF (STEP1_EN_BIT&amp;0x05)
 #define STEP1_EN_CR CRH
 #endif
 #define DIO9 9
@@ -1763,7 +1763,7 @@
 #define STEP2_EN_CROFF STEP2_EN_BIT
 #define STEP2_EN_CR CRL
 #else
-#define STEP2_EN_CROFF (STEP2_EN_BIT&amp;0x03)
+#define STEP2_EN_CROFF (STEP2_EN_BIT&amp;0x05)
 #define STEP2_EN_CR CRH
 #endif
 #define DIO10 10
@@ -1828,7 +1828,7 @@
 #define STEP3_EN_CROFF STEP3_EN_BIT
 #define STEP3_EN_CR CRL
 #else
-#define STEP3_EN_CROFF (STEP3_EN_BIT&amp;0x03)
+#define STEP3_EN_CROFF (STEP3_EN_BIT&amp;0x05)
 #define STEP3_EN_CR CRH
 #endif
 #define DIO11 11
@@ -1893,7 +1893,7 @@
 #define STEP4_EN_CROFF STEP4_EN_BIT
 #define STEP4_EN_CR CRL
 #else
-#define STEP4_EN_CROFF (STEP4_EN_BIT&amp;0x03)
+#define STEP4_EN_CROFF (STEP4_EN_BIT&amp;0x05)
 #define STEP4_EN_CR CRH
 #endif
 #define DIO12 12
@@ -1958,7 +1958,7 @@
 #define STEP5_EN_CROFF STEP5_EN_BIT
 #define STEP5_EN_CR CRL
 #else
-#define STEP5_EN_CROFF (STEP5_EN_BIT&amp;0x03)
+#define STEP5_EN_CROFF (STEP5_EN_BIT&amp;0x05)
 #define STEP5_EN_CR CRH
 #endif
 #define DIO13 13
@@ -2023,7 +2023,7 @@
 #define DIR0_CROFF DIR0_BIT
 #define DIR0_CR CRL
 #else
-#define DIR0_CROFF (DIR0_BIT&amp;0x03)
+#define DIR0_CROFF (DIR0_BIT&amp;0x05)
 #define DIR0_CR CRH
 #endif
 #define DIO14 14
@@ -2088,7 +2088,7 @@
 #define DIR1_CROFF DIR1_BIT
 #define DIR1_CR CRL
 #else
-#define DIR1_CROFF (DIR1_BIT&amp;0x03)
+#define DIR1_CROFF (DIR1_BIT&amp;0x05)
 #define DIR1_CR CRH
 #endif
 #define DIO15 15
@@ -2153,7 +2153,7 @@
 #define DIR2_CROFF DIR2_BIT
 #define DIR2_CR CRL
 #else
-#define DIR2_CROFF (DIR2_BIT&amp;0x03)
+#define DIR2_CROFF (DIR2_BIT&amp;0x05)
 #define DIR2_CR CRH
 #endif
 #define DIO16 16
@@ -2218,7 +2218,7 @@
 #define DIR3_CROFF DIR3_BIT
 #define DIR3_CR CRL
 #else
-#define DIR3_CROFF (DIR3_BIT&amp;0x03)
+#define DIR3_CROFF (DIR3_BIT&amp;0x05)
 #define DIR3_CR CRH
 #endif
 #define DIO17 17
@@ -2283,7 +2283,7 @@
 #define DIR4_CROFF DIR4_BIT
 #define DIR4_CR CRL
 #else
-#define DIR4_CROFF (DIR4_BIT&amp;0x03)
+#define DIR4_CROFF (DIR4_BIT&amp;0x05)
 #define DIR4_CR CRH
 #endif
 #define DIO18 18
@@ -2348,7 +2348,7 @@
 #define DIR5_CROFF DIR5_BIT
 #define DIR5_CR CRL
 #else
-#define DIR5_CROFF (DIR5_BIT&amp;0x03)
+#define DIR5_CROFF (DIR5_BIT&amp;0x05)
 #define DIR5_CR CRH
 #endif
 #define DIO19 19
@@ -2415,7 +2415,7 @@
 #define PWM0_CROFF PWM0_BIT
 #define PWM0_CR CRL
 #else
-#define PWM0_CROFF (PWM0_BIT&amp;0x03)
+#define PWM0_CROFF (PWM0_BIT&amp;0x05)
 #define PWM0_CR CRH
 #endif
 #define DIO20 20
@@ -2567,7 +2567,7 @@
 #define PWM1_CROFF PWM1_BIT
 #define PWM1_CR CRL
 #else
-#define PWM1_CROFF (PWM1_BIT&amp;0x03)
+#define PWM1_CROFF (PWM1_BIT&amp;0x05)
 #define PWM1_CR CRH
 #endif
 #define DIO21 21
@@ -2719,7 +2719,7 @@
 #define PWM2_CROFF PWM2_BIT
 #define PWM2_CR CRL
 #else
-#define PWM2_CROFF (PWM2_BIT&amp;0x03)
+#define PWM2_CROFF (PWM2_BIT&amp;0x05)
 #define PWM2_CR CRH
 #endif
 #define DIO22 22
@@ -2828,7 +2828,7 @@
 #define PWM3_CROFF PWM3_BIT
 #define PWM3_CR CRL
 #else
-#define PWM3_CROFF (PWM3_BIT&amp;0x03)
+#define PWM3_CROFF (PWM3_BIT&amp;0x05)
 #define PWM3_CR CRH
 #endif
 #define DIO23 23
@@ -2937,7 +2937,7 @@
 #define PWM4_CROFF PWM4_BIT
 #define PWM4_CR CRL
 #else
-#define PWM4_CROFF (PWM4_BIT&amp;0x03)
+#define PWM4_CROFF (PWM4_BIT&amp;0x05)
 #define PWM4_CR CRH
 #endif
 #define DIO24 24
@@ -3046,7 +3046,7 @@
 #define PWM5_CROFF PWM5_BIT
 #define PWM5_CR CRL
 #else
-#define PWM5_CROFF (PWM5_BIT&amp;0x03)
+#define PWM5_CROFF (PWM5_BIT&amp;0x05)
 #define PWM5_CR CRH
 #endif
 #define DIO25 25
@@ -3155,7 +3155,7 @@
 #define PWM6_CROFF PWM6_BIT
 #define PWM6_CR CRL
 #else
-#define PWM6_CROFF (PWM6_BIT&amp;0x03)
+#define PWM6_CROFF (PWM6_BIT&amp;0x05)
 #define PWM6_CR CRH
 #endif
 #define DIO26 26
@@ -3264,7 +3264,7 @@
 #define PWM7_CROFF PWM7_BIT
 #define PWM7_CR CRL
 #else
-#define PWM7_CROFF (PWM7_BIT&amp;0x03)
+#define PWM7_CROFF (PWM7_BIT&amp;0x05)
 #define PWM7_CR CRH
 #endif
 #define DIO27 27
@@ -3373,7 +3373,7 @@
 #define PWM8_CROFF PWM8_BIT
 #define PWM8_CR CRL
 #else
-#define PWM8_CROFF (PWM8_BIT&amp;0x03)
+#define PWM8_CROFF (PWM8_BIT&amp;0x05)
 #define PWM8_CR CRH
 #endif
 #define DIO28 28
@@ -3482,7 +3482,7 @@
 #define PWM9_CROFF PWM9_BIT
 #define PWM9_CR CRL
 #else
-#define PWM9_CROFF (PWM9_BIT&amp;0x03)
+#define PWM9_CROFF (PWM9_BIT&amp;0x05)
 #define PWM9_CR CRH
 #endif
 #define DIO29 29
@@ -3591,7 +3591,7 @@
 #define PWM10_CROFF PWM10_BIT
 #define PWM10_CR CRL
 #else
-#define PWM10_CROFF (PWM10_BIT&amp;0x03)
+#define PWM10_CROFF (PWM10_BIT&amp;0x05)
 #define PWM10_CR CRH
 #endif
 #define DIO30 30
@@ -3700,7 +3700,7 @@
 #define PWM11_CROFF PWM11_BIT
 #define PWM11_CR CRL
 #else
-#define PWM11_CROFF (PWM11_BIT&amp;0x03)
+#define PWM11_CROFF (PWM11_BIT&amp;0x05)
 #define PWM11_CR CRH
 #endif
 #define DIO31 31
@@ -3809,7 +3809,7 @@
 #define PWM12_CROFF PWM12_BIT
 #define PWM12_CR CRL
 #else
-#define PWM12_CROFF (PWM12_BIT&amp;0x03)
+#define PWM12_CROFF (PWM12_BIT&amp;0x05)
 #define PWM12_CR CRH
 #endif
 #define DIO32 32
@@ -3918,7 +3918,7 @@
 #define PWM13_CROFF PWM13_BIT
 #define PWM13_CR CRL
 #else
-#define PWM13_CROFF (PWM13_BIT&amp;0x03)
+#define PWM13_CROFF (PWM13_BIT&amp;0x05)
 #define PWM13_CR CRH
 #endif
 #define DIO33 33
@@ -4027,7 +4027,7 @@
 #define PWM14_CROFF PWM14_BIT
 #define PWM14_CR CRL
 #else
-#define PWM14_CROFF (PWM14_BIT&amp;0x03)
+#define PWM14_CROFF (PWM14_BIT&amp;0x05)
 #define PWM14_CR CRH
 #endif
 #define DIO34 34
@@ -4136,7 +4136,7 @@
 #define PWM15_CROFF PWM15_BIT
 #define PWM15_CR CRL
 #else
-#define PWM15_CROFF (PWM15_BIT&amp;0x03)
+#define PWM15_CROFF (PWM15_BIT&amp;0x05)
 #define PWM15_CR CRH
 #endif
 #define DIO35 35
@@ -4243,7 +4243,7 @@
 #define TX_CROFF TX_BIT
 #define TX_CR CRL
 #else
-#define TX_CROFF (TX_BIT&amp;0x03)
+#define TX_CROFF (TX_BIT&amp;0x05)
 #define TX_CR CRH
 #endif
 #define DIO36 36
@@ -4303,7 +4303,7 @@
 #define DOUT0_CROFF DOUT0_BIT
 #define DOUT0_CR CRL
 #else
-#define DOUT0_CROFF (DOUT0_BIT&amp;0x03)
+#define DOUT0_CROFF (DOUT0_BIT&amp;0x05)
 #define DOUT0_CR CRH
 #endif
 #define DIO37 37
@@ -4368,7 +4368,7 @@
 #define DOUT1_CROFF DOUT1_BIT
 #define DOUT1_CR CRL
 #else
-#define DOUT1_CROFF (DOUT1_BIT&amp;0x03)
+#define DOUT1_CROFF (DOUT1_BIT&amp;0x05)
 #define DOUT1_CR CRH
 #endif
 #define DIO38 38
@@ -4433,7 +4433,7 @@
 #define DOUT2_CROFF DOUT2_BIT
 #define DOUT2_CR CRL
 #else
-#define DOUT2_CROFF (DOUT2_BIT&amp;0x03)
+#define DOUT2_CROFF (DOUT2_BIT&amp;0x05)
 #define DOUT2_CR CRH
 #endif
 #define DIO39 39
@@ -4498,7 +4498,7 @@
 #define DOUT3_CROFF DOUT3_BIT
 #define DOUT3_CR CRL
 #else
-#define DOUT3_CROFF (DOUT3_BIT&amp;0x03)
+#define DOUT3_CROFF (DOUT3_BIT&amp;0x05)
 #define DOUT3_CR CRH
 #endif
 #define DIO40 40
@@ -4563,7 +4563,7 @@
 #define DOUT4_CROFF DOUT4_BIT
 #define DOUT4_CR CRL
 #else
-#define DOUT4_CROFF (DOUT4_BIT&amp;0x03)
+#define DOUT4_CROFF (DOUT4_BIT&amp;0x05)
 #define DOUT4_CR CRH
 #endif
 #define DIO41 41
@@ -4628,7 +4628,7 @@
 #define DOUT5_CROFF DOUT5_BIT
 #define DOUT5_CR CRL
 #else
-#define DOUT5_CROFF (DOUT5_BIT&amp;0x03)
+#define DOUT5_CROFF (DOUT5_BIT&amp;0x05)
 #define DOUT5_CR CRH
 #endif
 #define DIO42 42
@@ -4693,7 +4693,7 @@
 #define DOUT6_CROFF DOUT6_BIT
 #define DOUT6_CR CRL
 #else
-#define DOUT6_CROFF (DOUT6_BIT&amp;0x03)
+#define DOUT6_CROFF (DOUT6_BIT&amp;0x05)
 #define DOUT6_CR CRH
 #endif
 #define DIO43 43
@@ -4758,7 +4758,7 @@
 #define DOUT7_CROFF DOUT7_BIT
 #define DOUT7_CR CRL
 #else
-#define DOUT7_CROFF (DOUT7_BIT&amp;0x03)
+#define DOUT7_CROFF (DOUT7_BIT&amp;0x05)
 #define DOUT7_CR CRH
 #endif
 #define DIO44 44
@@ -4823,7 +4823,7 @@
 #define DOUT8_CROFF DOUT8_BIT
 #define DOUT8_CR CRL
 #else
-#define DOUT8_CROFF (DOUT8_BIT&amp;0x03)
+#define DOUT8_CROFF (DOUT8_BIT&amp;0x05)
 #define DOUT8_CR CRH
 #endif
 #define DIO45 45
@@ -4888,7 +4888,7 @@
 #define DOUT9_CROFF DOUT9_BIT
 #define DOUT9_CR CRL
 #else
-#define DOUT9_CROFF (DOUT9_BIT&amp;0x03)
+#define DOUT9_CROFF (DOUT9_BIT&amp;0x05)
 #define DOUT9_CR CRH
 #endif
 #define DIO46 46
@@ -4953,7 +4953,7 @@
 #define DOUT10_CROFF DOUT10_BIT
 #define DOUT10_CR CRL
 #else
-#define DOUT10_CROFF (DOUT10_BIT&amp;0x03)
+#define DOUT10_CROFF (DOUT10_BIT&amp;0x05)
 #define DOUT10_CR CRH
 #endif
 #define DIO47 47
@@ -5018,7 +5018,7 @@
 #define DOUT11_CROFF DOUT11_BIT
 #define DOUT11_CR CRL
 #else
-#define DOUT11_CROFF (DOUT11_BIT&amp;0x03)
+#define DOUT11_CROFF (DOUT11_BIT&amp;0x05)
 #define DOUT11_CR CRH
 #endif
 #define DIO48 48
@@ -5083,7 +5083,7 @@
 #define DOUT12_CROFF DOUT12_BIT
 #define DOUT12_CR CRL
 #else
-#define DOUT12_CROFF (DOUT12_BIT&amp;0x03)
+#define DOUT12_CROFF (DOUT12_BIT&amp;0x05)
 #define DOUT12_CR CRH
 #endif
 #define DIO49 49
@@ -5148,7 +5148,7 @@
 #define DOUT13_CROFF DOUT13_BIT
 #define DOUT13_CR CRL
 #else
-#define DOUT13_CROFF (DOUT13_BIT&amp;0x03)
+#define DOUT13_CROFF (DOUT13_BIT&amp;0x05)
 #define DOUT13_CR CRH
 #endif
 #define DIO50 50
@@ -5213,7 +5213,7 @@
 #define DOUT14_CROFF DOUT14_BIT
 #define DOUT14_CR CRL
 #else
-#define DOUT14_CROFF (DOUT14_BIT&amp;0x03)
+#define DOUT14_CROFF (DOUT14_BIT&amp;0x05)
 #define DOUT14_CR CRH
 #endif
 #define DIO51 51
@@ -5278,7 +5278,7 @@
 #define DOUT15_CROFF DOUT15_BIT
 #define DOUT15_CR CRL
 #else
-#define DOUT15_CROFF (DOUT15_BIT&amp;0x03)
+#define DOUT15_CROFF (DOUT15_BIT&amp;0x05)
 #define DOUT15_CR CRH
 #endif
 #define DIO52 52
@@ -5347,7 +5347,7 @@
 #define LIMIT_X_CROFF LIMIT_X_BIT
 #define LIMIT_X_CR CRL
 #else
-#define LIMIT_X_CROFF (LIMIT_X_BIT&amp;0x03)
+#define LIMIT_X_CROFF (LIMIT_X_BIT&amp;0x05)
 #define LIMIT_X_CR CRH
 #endif
 #define DIO53 53
@@ -5453,7 +5453,7 @@
 #define LIMIT_Y_CROFF LIMIT_Y_BIT
 #define LIMIT_Y_CR CRL
 #else
-#define LIMIT_Y_CROFF (LIMIT_Y_BIT&amp;0x03)
+#define LIMIT_Y_CROFF (LIMIT_Y_BIT&amp;0x05)
 #define LIMIT_Y_CR CRH
 #endif
 #define DIO54 54
@@ -5559,7 +5559,7 @@
 #define LIMIT_Z_CROFF LIMIT_Z_BIT
 #define LIMIT_Z_CR CRL
 #else
-#define LIMIT_Z_CROFF (LIMIT_Z_BIT&amp;0x03)
+#define LIMIT_Z_CROFF (LIMIT_Z_BIT&amp;0x05)
 #define LIMIT_Z_CR CRH
 #endif
 #define DIO55 55
@@ -5645,7 +5645,7 @@
 #define LIMIT_X2_CROFF LIMIT_X2_BIT
 #define LIMIT_X2_CR CRL
 #else
-#define LIMIT_X2_CROFF (LIMIT_X2_BIT&amp;0x03)
+#define LIMIT_X2_CROFF (LIMIT_X2_BIT&amp;0x05)
 #define LIMIT_X2_CR CRH
 #endif
 #define DIO56 56
@@ -5731,7 +5731,7 @@
 #define LIMIT_Y2_CROFF LIMIT_Y2_BIT
 #define LIMIT_Y2_CR CRL
 #else
-#define LIMIT_Y2_CROFF (LIMIT_Y2_BIT&amp;0x03)
+#define LIMIT_Y2_CROFF (LIMIT_Y2_BIT&amp;0x05)
 #define LIMIT_Y2_CR CRH
 #endif
 #define DIO57 57
@@ -5817,7 +5817,7 @@
 #define LIMIT_Z2_CROFF LIMIT_Z2_BIT
 #define LIMIT_Z2_CR CRL
 #else
-#define LIMIT_Z2_CROFF (LIMIT_Z2_BIT&amp;0x03)
+#define LIMIT_Z2_CROFF (LIMIT_Z2_BIT&amp;0x05)
 #define LIMIT_Z2_CR CRH
 #endif
 #define DIO58 58
@@ -5903,7 +5903,7 @@
 #define LIMIT_A_CROFF LIMIT_A_BIT
 #define LIMIT_A_CR CRL
 #else
-#define LIMIT_A_CROFF (LIMIT_A_BIT&amp;0x03)
+#define LIMIT_A_CROFF (LIMIT_A_BIT&amp;0x05)
 #define LIMIT_A_CR CRH
 #endif
 #define DIO59 59
@@ -5989,7 +5989,7 @@
 #define LIMIT_B_CROFF LIMIT_B_BIT
 #define LIMIT_B_CR CRL
 #else
-#define LIMIT_B_CROFF (LIMIT_B_BIT&amp;0x03)
+#define LIMIT_B_CROFF (LIMIT_B_BIT&amp;0x05)
 #define LIMIT_B_CR CRH
 #endif
 #define DIO60 60
@@ -6075,7 +6075,7 @@
 #define LIMIT_C_CROFF LIMIT_C_BIT
 #define LIMIT_C_CR CRL
 #else
-#define LIMIT_C_CROFF (LIMIT_C_BIT&amp;0x03)
+#define LIMIT_C_CROFF (LIMIT_C_BIT&amp;0x05)
 #define LIMIT_C_CR CRH
 #endif
 #define DIO61 61
@@ -6161,7 +6161,7 @@
 #define PROBE_CROFF PROBE_BIT
 #define PROBE_CR CRL
 #else
-#define PROBE_CROFF (PROBE_BIT&amp;0x03)
+#define PROBE_CROFF (PROBE_BIT&amp;0x05)
 #define PROBE_CR CRH
 #endif
 #define DIO62 62
@@ -6247,7 +6247,7 @@
 #define ESTOP_CROFF ESTOP_BIT
 #define ESTOP_CR CRL
 #else
-#define ESTOP_CROFF (ESTOP_BIT&amp;0x03)
+#define ESTOP_CROFF (ESTOP_BIT&amp;0x05)
 #define ESTOP_CR CRH
 #endif
 #define DIO63 63
@@ -6333,7 +6333,7 @@
 #define SAFETY_DOOR_CROFF SAFETY_DOOR_BIT
 #define SAFETY_DOOR_CR CRL
 #else
-#define SAFETY_DOOR_CROFF (SAFETY_DOOR_BIT&amp;0x03)
+#define SAFETY_DOOR_CROFF (SAFETY_DOOR_BIT&amp;0x05)
 #define SAFETY_DOOR_CR CRH
 #endif
 #define DIO64 64
@@ -6418,7 +6418,7 @@
 #define "&amp;C68&amp;"_CROFF "&amp;C68&amp;"_BIT
 #define "&amp;C68&amp;"_CR CRL
 #else
-#define "&amp;C68&amp;"_CROFF ("&amp;C68&amp;"_BIT&amp;0x03)
+#define "&amp;C68&amp;"_CROFF ("&amp;C68&amp;"_BIT&amp;0x05)
 #define "&amp;C68&amp;"_CR CRH
 #endif
 #define "&amp;B68&amp;" "&amp;A68&amp;"
@@ -6437,7 +6437,7 @@
 #define FHOLD_CROFF FHOLD_BIT
 #define FHOLD_CR CRL
 #else
-#define FHOLD_CROFF (FHOLD_BIT&amp;0x03)
+#define FHOLD_CROFF (FHOLD_BIT&amp;0x05)
 #define FHOLD_CR CRH
 #endif
 #define DIO65 65
@@ -6523,7 +6523,7 @@
 #define CS_RES_CROFF CS_RES_BIT
 #define CS_RES_CR CRL
 #else
-#define CS_RES_CROFF (CS_RES_BIT&amp;0x03)
+#define CS_RES_CROFF (CS_RES_BIT&amp;0x05)
 #define CS_RES_CR CRH
 #endif
 #define DIO66 66
@@ -6611,7 +6611,7 @@
 #define ANALOG0_CROFF ANALOG0_BIT
 #define ANALOG0_CR CRL
 #else
-#define ANALOG0_CROFF (ANALOG0_BIT&amp;0x03)
+#define ANALOG0_CROFF (ANALOG0_BIT&amp;0x05)
 #define ANALOG0_CR CRH
 #endif
 #define DIO67 67
@@ -6687,7 +6687,7 @@
 #define ANALOG1_CROFF ANALOG1_BIT
 #define ANALOG1_CR CRL
 #else
-#define ANALOG1_CROFF (ANALOG1_BIT&amp;0x03)
+#define ANALOG1_CROFF (ANALOG1_BIT&amp;0x05)
 #define ANALOG1_CR CRH
 #endif
 #define DIO68 68
@@ -6763,7 +6763,7 @@
 #define ANALOG2_CROFF ANALOG2_BIT
 #define ANALOG2_CR CRL
 #else
-#define ANALOG2_CROFF (ANALOG2_BIT&amp;0x03)
+#define ANALOG2_CROFF (ANALOG2_BIT&amp;0x05)
 #define ANALOG2_CR CRH
 #endif
 #define DIO69 69
@@ -6834,7 +6834,7 @@
 #define ANALOG3_CROFF ANALOG3_BIT
 #define ANALOG3_CR CRL
 #else
-#define ANALOG3_CROFF (ANALOG3_BIT&amp;0x03)
+#define ANALOG3_CROFF (ANALOG3_BIT&amp;0x05)
 #define ANALOG3_CR CRH
 #endif
 #define DIO70 70
@@ -6905,7 +6905,7 @@
 #define ANALOG4_CROFF ANALOG4_BIT
 #define ANALOG4_CR CRL
 #else
-#define ANALOG4_CROFF (ANALOG4_BIT&amp;0x03)
+#define ANALOG4_CROFF (ANALOG4_BIT&amp;0x05)
 #define ANALOG4_CR CRH
 #endif
 #define DIO71 71
@@ -6976,7 +6976,7 @@
 #define ANALOG5_CROFF ANALOG5_BIT
 #define ANALOG5_CR CRL
 #else
-#define ANALOG5_CROFF (ANALOG5_BIT&amp;0x03)
+#define ANALOG5_CROFF (ANALOG5_BIT&amp;0x05)
 #define ANALOG5_CR CRH
 #endif
 #define DIO72 72
@@ -7047,7 +7047,7 @@
 #define ANALOG6_CROFF ANALOG6_BIT
 #define ANALOG6_CR CRL
 #else
-#define ANALOG6_CROFF (ANALOG6_BIT&amp;0x03)
+#define ANALOG6_CROFF (ANALOG6_BIT&amp;0x05)
 #define ANALOG6_CR CRH
 #endif
 #define DIO73 73
@@ -7118,7 +7118,7 @@
 #define ANALOG7_CROFF ANALOG7_BIT
 #define ANALOG7_CR CRL
 #else
-#define ANALOG7_CROFF (ANALOG7_BIT&amp;0x03)
+#define ANALOG7_CROFF (ANALOG7_BIT&amp;0x05)
 #define ANALOG7_CR CRH
 #endif
 #define DIO74 74
@@ -7189,7 +7189,7 @@
 #define ANALOG8_CROFF ANALOG8_BIT
 #define ANALOG8_CR CRL
 #else
-#define ANALOG8_CROFF (ANALOG8_BIT&amp;0x03)
+#define ANALOG8_CROFF (ANALOG8_BIT&amp;0x05)
 #define ANALOG8_CR CRH
 #endif
 #define DIO75 75
@@ -7260,7 +7260,7 @@
 #define ANALOG9_CROFF ANALOG9_BIT
 #define ANALOG9_CR CRL
 #else
-#define ANALOG9_CROFF (ANALOG9_BIT&amp;0x03)
+#define ANALOG9_CROFF (ANALOG9_BIT&amp;0x05)
 #define ANALOG9_CR CRH
 #endif
 #define DIO76 76
@@ -7331,7 +7331,7 @@
 #define ANALOG10_CROFF ANALOG10_BIT
 #define ANALOG10_CR CRL
 #else
-#define ANALOG10_CROFF (ANALOG10_BIT&amp;0x03)
+#define ANALOG10_CROFF (ANALOG10_BIT&amp;0x05)
 #define ANALOG10_CR CRH
 #endif
 #define DIO77 77
@@ -7402,7 +7402,7 @@
 #define ANALOG11_CROFF ANALOG11_BIT
 #define ANALOG11_CR CRL
 #else
-#define ANALOG11_CROFF (ANALOG11_BIT&amp;0x03)
+#define ANALOG11_CROFF (ANALOG11_BIT&amp;0x05)
 #define ANALOG11_CR CRH
 #endif
 #define DIO78 78
@@ -7473,7 +7473,7 @@
 #define ANALOG12_CROFF ANALOG12_BIT
 #define ANALOG12_CR CRL
 #else
-#define ANALOG12_CROFF (ANALOG12_BIT&amp;0x03)
+#define ANALOG12_CROFF (ANALOG12_BIT&amp;0x05)
 #define ANALOG12_CR CRH
 #endif
 #define DIO79 79
@@ -7544,7 +7544,7 @@
 #define ANALOG13_CROFF ANALOG13_BIT
 #define ANALOG13_CR CRL
 #else
-#define ANALOG13_CROFF (ANALOG13_BIT&amp;0x03)
+#define ANALOG13_CROFF (ANALOG13_BIT&amp;0x05)
 #define ANALOG13_CR CRH
 #endif
 #define DIO80 80
@@ -7615,7 +7615,7 @@
 #define ANALOG14_CROFF ANALOG14_BIT
 #define ANALOG14_CR CRL
 #else
-#define ANALOG14_CROFF (ANALOG14_BIT&amp;0x03)
+#define ANALOG14_CROFF (ANALOG14_BIT&amp;0x05)
 #define ANALOG14_CR CRH
 #endif
 #define DIO81 81
@@ -7686,7 +7686,7 @@
 #define ANALOG15_CROFF ANALOG15_BIT
 #define ANALOG15_CR CRL
 #else
-#define ANALOG15_CROFF (ANALOG15_BIT&amp;0x03)
+#define ANALOG15_CROFF (ANALOG15_BIT&amp;0x05)
 #define ANALOG15_CR CRH
 #endif
 #define DIO82 82
@@ -7757,7 +7757,7 @@
 #define RX_CROFF RX_BIT
 #define RX_CR CRL
 #else
-#define RX_CROFF (RX_BIT&amp;0x03)
+#define RX_CROFF (RX_BIT&amp;0x05)
 #define RX_CR CRH
 #endif
 #define DIO83 83
@@ -7817,7 +7817,7 @@
 #define DIN0_CROFF DIN0_BIT
 #define DIN0_CR CRL
 #else
-#define DIN0_CROFF (DIN0_BIT&amp;0x03)
+#define DIN0_CROFF (DIN0_BIT&amp;0x05)
 #define DIN0_CR CRH
 #endif
 #define DIO84 84
@@ -7890,7 +7890,7 @@
 #define DIN1_CROFF DIN1_BIT
 #define DIN1_CR CRL
 #else
-#define DIN1_CROFF (DIN1_BIT&amp;0x03)
+#define DIN1_CROFF (DIN1_BIT&amp;0x05)
 #define DIN1_CR CRH
 #endif
 #define DIO85 85
@@ -7963,7 +7963,7 @@
 #define DIN2_CROFF DIN2_BIT
 #define DIN2_CR CRL
 #else
-#define DIN2_CROFF (DIN2_BIT&amp;0x03)
+#define DIN2_CROFF (DIN2_BIT&amp;0x05)
 #define DIN2_CR CRH
 #endif
 #define DIO86 86
@@ -8031,7 +8031,7 @@
 #define DIN3_CROFF DIN3_BIT
 #define DIN3_CR CRL
 #else
-#define DIN3_CROFF (DIN3_BIT&amp;0x03)
+#define DIN3_CROFF (DIN3_BIT&amp;0x05)
 #define DIN3_CR CRH
 #endif
 #define DIO87 87
@@ -8099,7 +8099,7 @@
 #define DIN4_CROFF DIN4_BIT
 #define DIN4_CR CRL
 #else
-#define DIN4_CROFF (DIN4_BIT&amp;0x03)
+#define DIN4_CROFF (DIN4_BIT&amp;0x05)
 #define DIN4_CR CRH
 #endif
 #define DIO88 88
@@ -8167,7 +8167,7 @@
 #define DIN5_CROFF DIN5_BIT
 #define DIN5_CR CRL
 #else
-#define DIN5_CROFF (DIN5_BIT&amp;0x03)
+#define DIN5_CROFF (DIN5_BIT&amp;0x05)
 #define DIN5_CR CRH
 #endif
 #define DIO89 89
@@ -8235,7 +8235,7 @@
 #define DIN6_CROFF DIN6_BIT
 #define DIN6_CR CRL
 #else
-#define DIN6_CROFF (DIN6_BIT&amp;0x03)
+#define DIN6_CROFF (DIN6_BIT&amp;0x05)
 #define DIN6_CR CRH
 #endif
 #define DIO90 90
@@ -8303,7 +8303,7 @@
 #define DIN7_CROFF DIN7_BIT
 #define DIN7_CR CRL
 #else
-#define DIN7_CROFF (DIN7_BIT&amp;0x03)
+#define DIN7_CROFF (DIN7_BIT&amp;0x05)
 #define DIN7_CR CRH
 #endif
 #define DIO91 91
@@ -8371,7 +8371,7 @@
 #define DIN8_CROFF DIN8_BIT
 #define DIN8_CR CRL
 #else
-#define DIN8_CROFF (DIN8_BIT&amp;0x03)
+#define DIN8_CROFF (DIN8_BIT&amp;0x05)
 #define DIN8_CR CRH
 #endif
 #define DIO92 92
@@ -8439,7 +8439,7 @@
 #define DIN9_CROFF DIN9_BIT
 #define DIN9_CR CRL
 #else
-#define DIN9_CROFF (DIN9_BIT&amp;0x03)
+#define DIN9_CROFF (DIN9_BIT&amp;0x05)
 #define DIN9_CR CRH
 #endif
 #define DIO93 93
@@ -8507,7 +8507,7 @@
 #define DIN10_CROFF DIN10_BIT
 #define DIN10_CR CRL
 #else
-#define DIN10_CROFF (DIN10_BIT&amp;0x03)
+#define DIN10_CROFF (DIN10_BIT&amp;0x05)
 #define DIN10_CR CRH
 #endif
 #define DIO94 94
@@ -8575,7 +8575,7 @@
 #define DIN11_CROFF DIN11_BIT
 #define DIN11_CR CRL
 #else
-#define DIN11_CROFF (DIN11_BIT&amp;0x03)
+#define DIN11_CROFF (DIN11_BIT&amp;0x05)
 #define DIN11_CR CRH
 #endif
 #define DIO95 95
@@ -8643,7 +8643,7 @@
 #define DIN12_CROFF DIN12_BIT
 #define DIN12_CR CRL
 #else
-#define DIN12_CROFF (DIN12_BIT&amp;0x03)
+#define DIN12_CROFF (DIN12_BIT&amp;0x05)
 #define DIN12_CR CRH
 #endif
 #define DIO96 96
@@ -8711,7 +8711,7 @@
 #define DIN13_CROFF DIN13_BIT
 #define DIN13_CR CRL
 #else
-#define DIN13_CROFF (DIN13_BIT&amp;0x03)
+#define DIN13_CROFF (DIN13_BIT&amp;0x05)
 #define DIN13_CR CRH
 #endif
 #define DIO97 97
@@ -8779,7 +8779,7 @@
 #define DIN14_CROFF DIN14_BIT
 #define DIN14_CR CRL
 #else
-#define DIN14_CROFF (DIN14_BIT&amp;0x03)
+#define DIN14_CROFF (DIN14_BIT&amp;0x05)
 #define DIN14_CR CRH
 #endif
 #define DIO98 98
@@ -8847,7 +8847,7 @@
 #define DIN15_CROFF DIN15_BIT
 #define DIN15_CR CRL
 #else
-#define DIN15_CROFF (DIN15_BIT&amp;0x03)
+#define DIN15_CROFF (DIN15_BIT&amp;0x05)
 #define DIN15_CR CRH
 #endif
 #define DIO99 99

</xml_diff>

<commit_message>
stm32 pin configuration fix
-fixed bug in the pin configuration macros helpers that caused the the pins not to be configured or get their configuration changed
</commit_message>
<xml_diff>
--- a/docs/stm32f1_mcumap_gen.xlsx
+++ b/docs/stm32f1_mcumap_gen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCEM\Documents\GitHub\uCNC\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AFCE7B-5A10-4E63-8916-2AF48D8A2359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D446E568-5890-4A6F-B9FD-1CE8783B1F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56:F69"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -870,7 +870,7 @@
 #define "&amp;C3&amp;"_CROFF "&amp;C3&amp;"_BIT
 #define "&amp;C3&amp;"_CR CRL
 #else
-#define "&amp;C3&amp;"_CROFF ("&amp;C3&amp;"_BIT&amp;0x03)
+#define "&amp;C3&amp;"_CROFF ("&amp;C3&amp;"_BIT&amp;0x05)
 #define "&amp;C3&amp;"_CR CRH
 #endif
 #define "&amp;B3&amp;" "&amp;A3&amp;"
@@ -889,7 +889,7 @@
 #define STEP0_CROFF STEP0_BIT
 #define STEP0_CR CRL
 #else
-#define STEP0_CROFF (STEP0_BIT&amp;0x03)
+#define STEP0_CROFF (STEP0_BIT&amp;0x05)
 #define STEP0_CR CRH
 #endif
 #define DIO0 0
@@ -990,7 +990,7 @@
 #define "&amp;C4&amp;"_CROFF "&amp;C4&amp;"_BIT
 #define "&amp;C4&amp;"_CR CRL
 #else
-#define "&amp;C4&amp;"_CROFF ("&amp;C4&amp;"_BIT&amp;0x03)
+#define "&amp;C4&amp;"_CROFF ("&amp;C4&amp;"_BIT&amp;0x05)
 #define "&amp;C4&amp;"_CR CRH
 #endif
 #define "&amp;B4&amp;" "&amp;A4&amp;"
@@ -1009,7 +1009,7 @@
 #define STEP1_CROFF STEP1_BIT
 #define STEP1_CR CRL
 #else
-#define STEP1_CROFF (STEP1_BIT&amp;0x03)
+#define STEP1_CROFF (STEP1_BIT&amp;0x05)
 #define STEP1_CR CRH
 #endif
 #define DIO1 1
@@ -1111,7 +1111,7 @@
 #define STEP2_CROFF STEP2_BIT
 #define STEP2_CR CRL
 #else
-#define STEP2_CROFF (STEP2_BIT&amp;0x03)
+#define STEP2_CROFF (STEP2_BIT&amp;0x05)
 #define STEP2_CR CRH
 #endif
 #define DIO2 2
@@ -1198,7 +1198,7 @@
 #define STEP3_CROFF STEP3_BIT
 #define STEP3_CR CRL
 #else
-#define STEP3_CROFF (STEP3_BIT&amp;0x03)
+#define STEP3_CROFF (STEP3_BIT&amp;0x05)
 #define STEP3_CR CRH
 #endif
 #define DIO3 3
@@ -1285,7 +1285,7 @@
 #define STEP4_CROFF STEP4_BIT
 #define STEP4_CR CRL
 #else
-#define STEP4_CROFF (STEP4_BIT&amp;0x03)
+#define STEP4_CROFF (STEP4_BIT&amp;0x05)
 #define STEP4_CR CRH
 #endif
 #define DIO4 4
@@ -1372,7 +1372,7 @@
 #define STEP5_CROFF STEP5_BIT
 #define STEP5_CR CRL
 #else
-#define STEP5_CROFF (STEP5_BIT&amp;0x03)
+#define STEP5_CROFF (STEP5_BIT&amp;0x05)
 #define STEP5_CR CRH
 #endif
 #define DIO5 5
@@ -1459,7 +1459,7 @@
 #define STEP6_CROFF STEP6_BIT
 #define STEP6_CR CRL
 #else
-#define STEP6_CROFF (STEP6_BIT&amp;0x03)
+#define STEP6_CROFF (STEP6_BIT&amp;0x05)
 #define STEP6_CR CRH
 #endif
 #define DIO6 6
@@ -1524,7 +1524,7 @@
 #define STEP7_CROFF STEP7_BIT
 #define STEP7_CR CRL
 #else
-#define STEP7_CROFF (STEP7_BIT&amp;0x03)
+#define STEP7_CROFF (STEP7_BIT&amp;0x05)
 #define STEP7_CR CRH
 #endif
 #define DIO7 7
@@ -1589,7 +1589,7 @@
 #define STEP0_EN_CROFF STEP0_EN_BIT
 #define STEP0_EN_CR CRL
 #else
-#define STEP0_EN_CROFF (STEP0_EN_BIT&amp;0x03)
+#define STEP0_EN_CROFF (STEP0_EN_BIT&amp;0x05)
 #define STEP0_EN_CR CRH
 #endif
 #define DIO8 8
@@ -1676,7 +1676,7 @@
 #define STEP1_EN_CROFF STEP1_EN_BIT
 #define STEP1_EN_CR CRL
 #else
-#define STEP1_EN_CROFF (STEP1_EN_BIT&amp;0x03)
+#define STEP1_EN_CROFF (STEP1_EN_BIT&amp;0x05)
 #define STEP1_EN_CR CRH
 #endif
 #define DIO9 9
@@ -1763,7 +1763,7 @@
 #define STEP2_EN_CROFF STEP2_EN_BIT
 #define STEP2_EN_CR CRL
 #else
-#define STEP2_EN_CROFF (STEP2_EN_BIT&amp;0x03)
+#define STEP2_EN_CROFF (STEP2_EN_BIT&amp;0x05)
 #define STEP2_EN_CR CRH
 #endif
 #define DIO10 10
@@ -1828,7 +1828,7 @@
 #define STEP3_EN_CROFF STEP3_EN_BIT
 #define STEP3_EN_CR CRL
 #else
-#define STEP3_EN_CROFF (STEP3_EN_BIT&amp;0x03)
+#define STEP3_EN_CROFF (STEP3_EN_BIT&amp;0x05)
 #define STEP3_EN_CR CRH
 #endif
 #define DIO11 11
@@ -1893,7 +1893,7 @@
 #define STEP4_EN_CROFF STEP4_EN_BIT
 #define STEP4_EN_CR CRL
 #else
-#define STEP4_EN_CROFF (STEP4_EN_BIT&amp;0x03)
+#define STEP4_EN_CROFF (STEP4_EN_BIT&amp;0x05)
 #define STEP4_EN_CR CRH
 #endif
 #define DIO12 12
@@ -1958,7 +1958,7 @@
 #define STEP5_EN_CROFF STEP5_EN_BIT
 #define STEP5_EN_CR CRL
 #else
-#define STEP5_EN_CROFF (STEP5_EN_BIT&amp;0x03)
+#define STEP5_EN_CROFF (STEP5_EN_BIT&amp;0x05)
 #define STEP5_EN_CR CRH
 #endif
 #define DIO13 13
@@ -2023,7 +2023,7 @@
 #define DIR0_CROFF DIR0_BIT
 #define DIR0_CR CRL
 #else
-#define DIR0_CROFF (DIR0_BIT&amp;0x03)
+#define DIR0_CROFF (DIR0_BIT&amp;0x05)
 #define DIR0_CR CRH
 #endif
 #define DIO14 14
@@ -2088,7 +2088,7 @@
 #define DIR1_CROFF DIR1_BIT
 #define DIR1_CR CRL
 #else
-#define DIR1_CROFF (DIR1_BIT&amp;0x03)
+#define DIR1_CROFF (DIR1_BIT&amp;0x05)
 #define DIR1_CR CRH
 #endif
 #define DIO15 15
@@ -2153,7 +2153,7 @@
 #define DIR2_CROFF DIR2_BIT
 #define DIR2_CR CRL
 #else
-#define DIR2_CROFF (DIR2_BIT&amp;0x03)
+#define DIR2_CROFF (DIR2_BIT&amp;0x05)
 #define DIR2_CR CRH
 #endif
 #define DIO16 16
@@ -2218,7 +2218,7 @@
 #define DIR3_CROFF DIR3_BIT
 #define DIR3_CR CRL
 #else
-#define DIR3_CROFF (DIR3_BIT&amp;0x03)
+#define DIR3_CROFF (DIR3_BIT&amp;0x05)
 #define DIR3_CR CRH
 #endif
 #define DIO17 17
@@ -2283,7 +2283,7 @@
 #define DIR4_CROFF DIR4_BIT
 #define DIR4_CR CRL
 #else
-#define DIR4_CROFF (DIR4_BIT&amp;0x03)
+#define DIR4_CROFF (DIR4_BIT&amp;0x05)
 #define DIR4_CR CRH
 #endif
 #define DIO18 18
@@ -2348,7 +2348,7 @@
 #define DIR5_CROFF DIR5_BIT
 #define DIR5_CR CRL
 #else
-#define DIR5_CROFF (DIR5_BIT&amp;0x03)
+#define DIR5_CROFF (DIR5_BIT&amp;0x05)
 #define DIR5_CR CRH
 #endif
 #define DIO19 19
@@ -2415,7 +2415,7 @@
 #define PWM0_CROFF PWM0_BIT
 #define PWM0_CR CRL
 #else
-#define PWM0_CROFF (PWM0_BIT&amp;0x03)
+#define PWM0_CROFF (PWM0_BIT&amp;0x05)
 #define PWM0_CR CRH
 #endif
 #define DIO20 20
@@ -2567,7 +2567,7 @@
 #define PWM1_CROFF PWM1_BIT
 #define PWM1_CR CRL
 #else
-#define PWM1_CROFF (PWM1_BIT&amp;0x03)
+#define PWM1_CROFF (PWM1_BIT&amp;0x05)
 #define PWM1_CR CRH
 #endif
 #define DIO21 21
@@ -2719,7 +2719,7 @@
 #define PWM2_CROFF PWM2_BIT
 #define PWM2_CR CRL
 #else
-#define PWM2_CROFF (PWM2_BIT&amp;0x03)
+#define PWM2_CROFF (PWM2_BIT&amp;0x05)
 #define PWM2_CR CRH
 #endif
 #define DIO22 22
@@ -2828,7 +2828,7 @@
 #define PWM3_CROFF PWM3_BIT
 #define PWM3_CR CRL
 #else
-#define PWM3_CROFF (PWM3_BIT&amp;0x03)
+#define PWM3_CROFF (PWM3_BIT&amp;0x05)
 #define PWM3_CR CRH
 #endif
 #define DIO23 23
@@ -2937,7 +2937,7 @@
 #define PWM4_CROFF PWM4_BIT
 #define PWM4_CR CRL
 #else
-#define PWM4_CROFF (PWM4_BIT&amp;0x03)
+#define PWM4_CROFF (PWM4_BIT&amp;0x05)
 #define PWM4_CR CRH
 #endif
 #define DIO24 24
@@ -3046,7 +3046,7 @@
 #define PWM5_CROFF PWM5_BIT
 #define PWM5_CR CRL
 #else
-#define PWM5_CROFF (PWM5_BIT&amp;0x03)
+#define PWM5_CROFF (PWM5_BIT&amp;0x05)
 #define PWM5_CR CRH
 #endif
 #define DIO25 25
@@ -3155,7 +3155,7 @@
 #define PWM6_CROFF PWM6_BIT
 #define PWM6_CR CRL
 #else
-#define PWM6_CROFF (PWM6_BIT&amp;0x03)
+#define PWM6_CROFF (PWM6_BIT&amp;0x05)
 #define PWM6_CR CRH
 #endif
 #define DIO26 26
@@ -3264,7 +3264,7 @@
 #define PWM7_CROFF PWM7_BIT
 #define PWM7_CR CRL
 #else
-#define PWM7_CROFF (PWM7_BIT&amp;0x03)
+#define PWM7_CROFF (PWM7_BIT&amp;0x05)
 #define PWM7_CR CRH
 #endif
 #define DIO27 27
@@ -3373,7 +3373,7 @@
 #define PWM8_CROFF PWM8_BIT
 #define PWM8_CR CRL
 #else
-#define PWM8_CROFF (PWM8_BIT&amp;0x03)
+#define PWM8_CROFF (PWM8_BIT&amp;0x05)
 #define PWM8_CR CRH
 #endif
 #define DIO28 28
@@ -3482,7 +3482,7 @@
 #define PWM9_CROFF PWM9_BIT
 #define PWM9_CR CRL
 #else
-#define PWM9_CROFF (PWM9_BIT&amp;0x03)
+#define PWM9_CROFF (PWM9_BIT&amp;0x05)
 #define PWM9_CR CRH
 #endif
 #define DIO29 29
@@ -3591,7 +3591,7 @@
 #define PWM10_CROFF PWM10_BIT
 #define PWM10_CR CRL
 #else
-#define PWM10_CROFF (PWM10_BIT&amp;0x03)
+#define PWM10_CROFF (PWM10_BIT&amp;0x05)
 #define PWM10_CR CRH
 #endif
 #define DIO30 30
@@ -3700,7 +3700,7 @@
 #define PWM11_CROFF PWM11_BIT
 #define PWM11_CR CRL
 #else
-#define PWM11_CROFF (PWM11_BIT&amp;0x03)
+#define PWM11_CROFF (PWM11_BIT&amp;0x05)
 #define PWM11_CR CRH
 #endif
 #define DIO31 31
@@ -3809,7 +3809,7 @@
 #define PWM12_CROFF PWM12_BIT
 #define PWM12_CR CRL
 #else
-#define PWM12_CROFF (PWM12_BIT&amp;0x03)
+#define PWM12_CROFF (PWM12_BIT&amp;0x05)
 #define PWM12_CR CRH
 #endif
 #define DIO32 32
@@ -3918,7 +3918,7 @@
 #define PWM13_CROFF PWM13_BIT
 #define PWM13_CR CRL
 #else
-#define PWM13_CROFF (PWM13_BIT&amp;0x03)
+#define PWM13_CROFF (PWM13_BIT&amp;0x05)
 #define PWM13_CR CRH
 #endif
 #define DIO33 33
@@ -4027,7 +4027,7 @@
 #define PWM14_CROFF PWM14_BIT
 #define PWM14_CR CRL
 #else
-#define PWM14_CROFF (PWM14_BIT&amp;0x03)
+#define PWM14_CROFF (PWM14_BIT&amp;0x05)
 #define PWM14_CR CRH
 #endif
 #define DIO34 34
@@ -4136,7 +4136,7 @@
 #define PWM15_CROFF PWM15_BIT
 #define PWM15_CR CRL
 #else
-#define PWM15_CROFF (PWM15_BIT&amp;0x03)
+#define PWM15_CROFF (PWM15_BIT&amp;0x05)
 #define PWM15_CR CRH
 #endif
 #define DIO35 35
@@ -4243,7 +4243,7 @@
 #define TX_CROFF TX_BIT
 #define TX_CR CRL
 #else
-#define TX_CROFF (TX_BIT&amp;0x03)
+#define TX_CROFF (TX_BIT&amp;0x05)
 #define TX_CR CRH
 #endif
 #define DIO36 36
@@ -4303,7 +4303,7 @@
 #define DOUT0_CROFF DOUT0_BIT
 #define DOUT0_CR CRL
 #else
-#define DOUT0_CROFF (DOUT0_BIT&amp;0x03)
+#define DOUT0_CROFF (DOUT0_BIT&amp;0x05)
 #define DOUT0_CR CRH
 #endif
 #define DIO37 37
@@ -4368,7 +4368,7 @@
 #define DOUT1_CROFF DOUT1_BIT
 #define DOUT1_CR CRL
 #else
-#define DOUT1_CROFF (DOUT1_BIT&amp;0x03)
+#define DOUT1_CROFF (DOUT1_BIT&amp;0x05)
 #define DOUT1_CR CRH
 #endif
 #define DIO38 38
@@ -4433,7 +4433,7 @@
 #define DOUT2_CROFF DOUT2_BIT
 #define DOUT2_CR CRL
 #else
-#define DOUT2_CROFF (DOUT2_BIT&amp;0x03)
+#define DOUT2_CROFF (DOUT2_BIT&amp;0x05)
 #define DOUT2_CR CRH
 #endif
 #define DIO39 39
@@ -4498,7 +4498,7 @@
 #define DOUT3_CROFF DOUT3_BIT
 #define DOUT3_CR CRL
 #else
-#define DOUT3_CROFF (DOUT3_BIT&amp;0x03)
+#define DOUT3_CROFF (DOUT3_BIT&amp;0x05)
 #define DOUT3_CR CRH
 #endif
 #define DIO40 40
@@ -4563,7 +4563,7 @@
 #define DOUT4_CROFF DOUT4_BIT
 #define DOUT4_CR CRL
 #else
-#define DOUT4_CROFF (DOUT4_BIT&amp;0x03)
+#define DOUT4_CROFF (DOUT4_BIT&amp;0x05)
 #define DOUT4_CR CRH
 #endif
 #define DIO41 41
@@ -4628,7 +4628,7 @@
 #define DOUT5_CROFF DOUT5_BIT
 #define DOUT5_CR CRL
 #else
-#define DOUT5_CROFF (DOUT5_BIT&amp;0x03)
+#define DOUT5_CROFF (DOUT5_BIT&amp;0x05)
 #define DOUT5_CR CRH
 #endif
 #define DIO42 42
@@ -4693,7 +4693,7 @@
 #define DOUT6_CROFF DOUT6_BIT
 #define DOUT6_CR CRL
 #else
-#define DOUT6_CROFF (DOUT6_BIT&amp;0x03)
+#define DOUT6_CROFF (DOUT6_BIT&amp;0x05)
 #define DOUT6_CR CRH
 #endif
 #define DIO43 43
@@ -4758,7 +4758,7 @@
 #define DOUT7_CROFF DOUT7_BIT
 #define DOUT7_CR CRL
 #else
-#define DOUT7_CROFF (DOUT7_BIT&amp;0x03)
+#define DOUT7_CROFF (DOUT7_BIT&amp;0x05)
 #define DOUT7_CR CRH
 #endif
 #define DIO44 44
@@ -4823,7 +4823,7 @@
 #define DOUT8_CROFF DOUT8_BIT
 #define DOUT8_CR CRL
 #else
-#define DOUT8_CROFF (DOUT8_BIT&amp;0x03)
+#define DOUT8_CROFF (DOUT8_BIT&amp;0x05)
 #define DOUT8_CR CRH
 #endif
 #define DIO45 45
@@ -4888,7 +4888,7 @@
 #define DOUT9_CROFF DOUT9_BIT
 #define DOUT9_CR CRL
 #else
-#define DOUT9_CROFF (DOUT9_BIT&amp;0x03)
+#define DOUT9_CROFF (DOUT9_BIT&amp;0x05)
 #define DOUT9_CR CRH
 #endif
 #define DIO46 46
@@ -4953,7 +4953,7 @@
 #define DOUT10_CROFF DOUT10_BIT
 #define DOUT10_CR CRL
 #else
-#define DOUT10_CROFF (DOUT10_BIT&amp;0x03)
+#define DOUT10_CROFF (DOUT10_BIT&amp;0x05)
 #define DOUT10_CR CRH
 #endif
 #define DIO47 47
@@ -5018,7 +5018,7 @@
 #define DOUT11_CROFF DOUT11_BIT
 #define DOUT11_CR CRL
 #else
-#define DOUT11_CROFF (DOUT11_BIT&amp;0x03)
+#define DOUT11_CROFF (DOUT11_BIT&amp;0x05)
 #define DOUT11_CR CRH
 #endif
 #define DIO48 48
@@ -5083,7 +5083,7 @@
 #define DOUT12_CROFF DOUT12_BIT
 #define DOUT12_CR CRL
 #else
-#define DOUT12_CROFF (DOUT12_BIT&amp;0x03)
+#define DOUT12_CROFF (DOUT12_BIT&amp;0x05)
 #define DOUT12_CR CRH
 #endif
 #define DIO49 49
@@ -5148,7 +5148,7 @@
 #define DOUT13_CROFF DOUT13_BIT
 #define DOUT13_CR CRL
 #else
-#define DOUT13_CROFF (DOUT13_BIT&amp;0x03)
+#define DOUT13_CROFF (DOUT13_BIT&amp;0x05)
 #define DOUT13_CR CRH
 #endif
 #define DIO50 50
@@ -5213,7 +5213,7 @@
 #define DOUT14_CROFF DOUT14_BIT
 #define DOUT14_CR CRL
 #else
-#define DOUT14_CROFF (DOUT14_BIT&amp;0x03)
+#define DOUT14_CROFF (DOUT14_BIT&amp;0x05)
 #define DOUT14_CR CRH
 #endif
 #define DIO51 51
@@ -5278,7 +5278,7 @@
 #define DOUT15_CROFF DOUT15_BIT
 #define DOUT15_CR CRL
 #else
-#define DOUT15_CROFF (DOUT15_BIT&amp;0x03)
+#define DOUT15_CROFF (DOUT15_BIT&amp;0x05)
 #define DOUT15_CR CRH
 #endif
 #define DIO52 52
@@ -5347,7 +5347,7 @@
 #define LIMIT_X_CROFF LIMIT_X_BIT
 #define LIMIT_X_CR CRL
 #else
-#define LIMIT_X_CROFF (LIMIT_X_BIT&amp;0x03)
+#define LIMIT_X_CROFF (LIMIT_X_BIT&amp;0x05)
 #define LIMIT_X_CR CRH
 #endif
 #define DIO53 53
@@ -5453,7 +5453,7 @@
 #define LIMIT_Y_CROFF LIMIT_Y_BIT
 #define LIMIT_Y_CR CRL
 #else
-#define LIMIT_Y_CROFF (LIMIT_Y_BIT&amp;0x03)
+#define LIMIT_Y_CROFF (LIMIT_Y_BIT&amp;0x05)
 #define LIMIT_Y_CR CRH
 #endif
 #define DIO54 54
@@ -5559,7 +5559,7 @@
 #define LIMIT_Z_CROFF LIMIT_Z_BIT
 #define LIMIT_Z_CR CRL
 #else
-#define LIMIT_Z_CROFF (LIMIT_Z_BIT&amp;0x03)
+#define LIMIT_Z_CROFF (LIMIT_Z_BIT&amp;0x05)
 #define LIMIT_Z_CR CRH
 #endif
 #define DIO55 55
@@ -5645,7 +5645,7 @@
 #define LIMIT_X2_CROFF LIMIT_X2_BIT
 #define LIMIT_X2_CR CRL
 #else
-#define LIMIT_X2_CROFF (LIMIT_X2_BIT&amp;0x03)
+#define LIMIT_X2_CROFF (LIMIT_X2_BIT&amp;0x05)
 #define LIMIT_X2_CR CRH
 #endif
 #define DIO56 56
@@ -5731,7 +5731,7 @@
 #define LIMIT_Y2_CROFF LIMIT_Y2_BIT
 #define LIMIT_Y2_CR CRL
 #else
-#define LIMIT_Y2_CROFF (LIMIT_Y2_BIT&amp;0x03)
+#define LIMIT_Y2_CROFF (LIMIT_Y2_BIT&amp;0x05)
 #define LIMIT_Y2_CR CRH
 #endif
 #define DIO57 57
@@ -5817,7 +5817,7 @@
 #define LIMIT_Z2_CROFF LIMIT_Z2_BIT
 #define LIMIT_Z2_CR CRL
 #else
-#define LIMIT_Z2_CROFF (LIMIT_Z2_BIT&amp;0x03)
+#define LIMIT_Z2_CROFF (LIMIT_Z2_BIT&amp;0x05)
 #define LIMIT_Z2_CR CRH
 #endif
 #define DIO58 58
@@ -5903,7 +5903,7 @@
 #define LIMIT_A_CROFF LIMIT_A_BIT
 #define LIMIT_A_CR CRL
 #else
-#define LIMIT_A_CROFF (LIMIT_A_BIT&amp;0x03)
+#define LIMIT_A_CROFF (LIMIT_A_BIT&amp;0x05)
 #define LIMIT_A_CR CRH
 #endif
 #define DIO59 59
@@ -5989,7 +5989,7 @@
 #define LIMIT_B_CROFF LIMIT_B_BIT
 #define LIMIT_B_CR CRL
 #else
-#define LIMIT_B_CROFF (LIMIT_B_BIT&amp;0x03)
+#define LIMIT_B_CROFF (LIMIT_B_BIT&amp;0x05)
 #define LIMIT_B_CR CRH
 #endif
 #define DIO60 60
@@ -6075,7 +6075,7 @@
 #define LIMIT_C_CROFF LIMIT_C_BIT
 #define LIMIT_C_CR CRL
 #else
-#define LIMIT_C_CROFF (LIMIT_C_BIT&amp;0x03)
+#define LIMIT_C_CROFF (LIMIT_C_BIT&amp;0x05)
 #define LIMIT_C_CR CRH
 #endif
 #define DIO61 61
@@ -6161,7 +6161,7 @@
 #define PROBE_CROFF PROBE_BIT
 #define PROBE_CR CRL
 #else
-#define PROBE_CROFF (PROBE_BIT&amp;0x03)
+#define PROBE_CROFF (PROBE_BIT&amp;0x05)
 #define PROBE_CR CRH
 #endif
 #define DIO62 62
@@ -6247,7 +6247,7 @@
 #define ESTOP_CROFF ESTOP_BIT
 #define ESTOP_CR CRL
 #else
-#define ESTOP_CROFF (ESTOP_BIT&amp;0x03)
+#define ESTOP_CROFF (ESTOP_BIT&amp;0x05)
 #define ESTOP_CR CRH
 #endif
 #define DIO63 63
@@ -6333,7 +6333,7 @@
 #define SAFETY_DOOR_CROFF SAFETY_DOOR_BIT
 #define SAFETY_DOOR_CR CRL
 #else
-#define SAFETY_DOOR_CROFF (SAFETY_DOOR_BIT&amp;0x03)
+#define SAFETY_DOOR_CROFF (SAFETY_DOOR_BIT&amp;0x05)
 #define SAFETY_DOOR_CR CRH
 #endif
 #define DIO64 64
@@ -6418,7 +6418,7 @@
 #define "&amp;C68&amp;"_CROFF "&amp;C68&amp;"_BIT
 #define "&amp;C68&amp;"_CR CRL
 #else
-#define "&amp;C68&amp;"_CROFF ("&amp;C68&amp;"_BIT&amp;0x03)
+#define "&amp;C68&amp;"_CROFF ("&amp;C68&amp;"_BIT&amp;0x05)
 #define "&amp;C68&amp;"_CR CRH
 #endif
 #define "&amp;B68&amp;" "&amp;A68&amp;"
@@ -6437,7 +6437,7 @@
 #define FHOLD_CROFF FHOLD_BIT
 #define FHOLD_CR CRL
 #else
-#define FHOLD_CROFF (FHOLD_BIT&amp;0x03)
+#define FHOLD_CROFF (FHOLD_BIT&amp;0x05)
 #define FHOLD_CR CRH
 #endif
 #define DIO65 65
@@ -6523,7 +6523,7 @@
 #define CS_RES_CROFF CS_RES_BIT
 #define CS_RES_CR CRL
 #else
-#define CS_RES_CROFF (CS_RES_BIT&amp;0x03)
+#define CS_RES_CROFF (CS_RES_BIT&amp;0x05)
 #define CS_RES_CR CRH
 #endif
 #define DIO66 66
@@ -6611,7 +6611,7 @@
 #define ANALOG0_CROFF ANALOG0_BIT
 #define ANALOG0_CR CRL
 #else
-#define ANALOG0_CROFF (ANALOG0_BIT&amp;0x03)
+#define ANALOG0_CROFF (ANALOG0_BIT&amp;0x05)
 #define ANALOG0_CR CRH
 #endif
 #define DIO67 67
@@ -6687,7 +6687,7 @@
 #define ANALOG1_CROFF ANALOG1_BIT
 #define ANALOG1_CR CRL
 #else
-#define ANALOG1_CROFF (ANALOG1_BIT&amp;0x03)
+#define ANALOG1_CROFF (ANALOG1_BIT&amp;0x05)
 #define ANALOG1_CR CRH
 #endif
 #define DIO68 68
@@ -6763,7 +6763,7 @@
 #define ANALOG2_CROFF ANALOG2_BIT
 #define ANALOG2_CR CRL
 #else
-#define ANALOG2_CROFF (ANALOG2_BIT&amp;0x03)
+#define ANALOG2_CROFF (ANALOG2_BIT&amp;0x05)
 #define ANALOG2_CR CRH
 #endif
 #define DIO69 69
@@ -6834,7 +6834,7 @@
 #define ANALOG3_CROFF ANALOG3_BIT
 #define ANALOG3_CR CRL
 #else
-#define ANALOG3_CROFF (ANALOG3_BIT&amp;0x03)
+#define ANALOG3_CROFF (ANALOG3_BIT&amp;0x05)
 #define ANALOG3_CR CRH
 #endif
 #define DIO70 70
@@ -6905,7 +6905,7 @@
 #define ANALOG4_CROFF ANALOG4_BIT
 #define ANALOG4_CR CRL
 #else
-#define ANALOG4_CROFF (ANALOG4_BIT&amp;0x03)
+#define ANALOG4_CROFF (ANALOG4_BIT&amp;0x05)
 #define ANALOG4_CR CRH
 #endif
 #define DIO71 71
@@ -6976,7 +6976,7 @@
 #define ANALOG5_CROFF ANALOG5_BIT
 #define ANALOG5_CR CRL
 #else
-#define ANALOG5_CROFF (ANALOG5_BIT&amp;0x03)
+#define ANALOG5_CROFF (ANALOG5_BIT&amp;0x05)
 #define ANALOG5_CR CRH
 #endif
 #define DIO72 72
@@ -7047,7 +7047,7 @@
 #define ANALOG6_CROFF ANALOG6_BIT
 #define ANALOG6_CR CRL
 #else
-#define ANALOG6_CROFF (ANALOG6_BIT&amp;0x03)
+#define ANALOG6_CROFF (ANALOG6_BIT&amp;0x05)
 #define ANALOG6_CR CRH
 #endif
 #define DIO73 73
@@ -7118,7 +7118,7 @@
 #define ANALOG7_CROFF ANALOG7_BIT
 #define ANALOG7_CR CRL
 #else
-#define ANALOG7_CROFF (ANALOG7_BIT&amp;0x03)
+#define ANALOG7_CROFF (ANALOG7_BIT&amp;0x05)
 #define ANALOG7_CR CRH
 #endif
 #define DIO74 74
@@ -7189,7 +7189,7 @@
 #define ANALOG8_CROFF ANALOG8_BIT
 #define ANALOG8_CR CRL
 #else
-#define ANALOG8_CROFF (ANALOG8_BIT&amp;0x03)
+#define ANALOG8_CROFF (ANALOG8_BIT&amp;0x05)
 #define ANALOG8_CR CRH
 #endif
 #define DIO75 75
@@ -7260,7 +7260,7 @@
 #define ANALOG9_CROFF ANALOG9_BIT
 #define ANALOG9_CR CRL
 #else
-#define ANALOG9_CROFF (ANALOG9_BIT&amp;0x03)
+#define ANALOG9_CROFF (ANALOG9_BIT&amp;0x05)
 #define ANALOG9_CR CRH
 #endif
 #define DIO76 76
@@ -7331,7 +7331,7 @@
 #define ANALOG10_CROFF ANALOG10_BIT
 #define ANALOG10_CR CRL
 #else
-#define ANALOG10_CROFF (ANALOG10_BIT&amp;0x03)
+#define ANALOG10_CROFF (ANALOG10_BIT&amp;0x05)
 #define ANALOG10_CR CRH
 #endif
 #define DIO77 77
@@ -7402,7 +7402,7 @@
 #define ANALOG11_CROFF ANALOG11_BIT
 #define ANALOG11_CR CRL
 #else
-#define ANALOG11_CROFF (ANALOG11_BIT&amp;0x03)
+#define ANALOG11_CROFF (ANALOG11_BIT&amp;0x05)
 #define ANALOG11_CR CRH
 #endif
 #define DIO78 78
@@ -7473,7 +7473,7 @@
 #define ANALOG12_CROFF ANALOG12_BIT
 #define ANALOG12_CR CRL
 #else
-#define ANALOG12_CROFF (ANALOG12_BIT&amp;0x03)
+#define ANALOG12_CROFF (ANALOG12_BIT&amp;0x05)
 #define ANALOG12_CR CRH
 #endif
 #define DIO79 79
@@ -7544,7 +7544,7 @@
 #define ANALOG13_CROFF ANALOG13_BIT
 #define ANALOG13_CR CRL
 #else
-#define ANALOG13_CROFF (ANALOG13_BIT&amp;0x03)
+#define ANALOG13_CROFF (ANALOG13_BIT&amp;0x05)
 #define ANALOG13_CR CRH
 #endif
 #define DIO80 80
@@ -7615,7 +7615,7 @@
 #define ANALOG14_CROFF ANALOG14_BIT
 #define ANALOG14_CR CRL
 #else
-#define ANALOG14_CROFF (ANALOG14_BIT&amp;0x03)
+#define ANALOG14_CROFF (ANALOG14_BIT&amp;0x05)
 #define ANALOG14_CR CRH
 #endif
 #define DIO81 81
@@ -7686,7 +7686,7 @@
 #define ANALOG15_CROFF ANALOG15_BIT
 #define ANALOG15_CR CRL
 #else
-#define ANALOG15_CROFF (ANALOG15_BIT&amp;0x03)
+#define ANALOG15_CROFF (ANALOG15_BIT&amp;0x05)
 #define ANALOG15_CR CRH
 #endif
 #define DIO82 82
@@ -7757,7 +7757,7 @@
 #define RX_CROFF RX_BIT
 #define RX_CR CRL
 #else
-#define RX_CROFF (RX_BIT&amp;0x03)
+#define RX_CROFF (RX_BIT&amp;0x05)
 #define RX_CR CRH
 #endif
 #define DIO83 83
@@ -7817,7 +7817,7 @@
 #define DIN0_CROFF DIN0_BIT
 #define DIN0_CR CRL
 #else
-#define DIN0_CROFF (DIN0_BIT&amp;0x03)
+#define DIN0_CROFF (DIN0_BIT&amp;0x05)
 #define DIN0_CR CRH
 #endif
 #define DIO84 84
@@ -7890,7 +7890,7 @@
 #define DIN1_CROFF DIN1_BIT
 #define DIN1_CR CRL
 #else
-#define DIN1_CROFF (DIN1_BIT&amp;0x03)
+#define DIN1_CROFF (DIN1_BIT&amp;0x05)
 #define DIN1_CR CRH
 #endif
 #define DIO85 85
@@ -7963,7 +7963,7 @@
 #define DIN2_CROFF DIN2_BIT
 #define DIN2_CR CRL
 #else
-#define DIN2_CROFF (DIN2_BIT&amp;0x03)
+#define DIN2_CROFF (DIN2_BIT&amp;0x05)
 #define DIN2_CR CRH
 #endif
 #define DIO86 86
@@ -8031,7 +8031,7 @@
 #define DIN3_CROFF DIN3_BIT
 #define DIN3_CR CRL
 #else
-#define DIN3_CROFF (DIN3_BIT&amp;0x03)
+#define DIN3_CROFF (DIN3_BIT&amp;0x05)
 #define DIN3_CR CRH
 #endif
 #define DIO87 87
@@ -8099,7 +8099,7 @@
 #define DIN4_CROFF DIN4_BIT
 #define DIN4_CR CRL
 #else
-#define DIN4_CROFF (DIN4_BIT&amp;0x03)
+#define DIN4_CROFF (DIN4_BIT&amp;0x05)
 #define DIN4_CR CRH
 #endif
 #define DIO88 88
@@ -8167,7 +8167,7 @@
 #define DIN5_CROFF DIN5_BIT
 #define DIN5_CR CRL
 #else
-#define DIN5_CROFF (DIN5_BIT&amp;0x03)
+#define DIN5_CROFF (DIN5_BIT&amp;0x05)
 #define DIN5_CR CRH
 #endif
 #define DIO89 89
@@ -8235,7 +8235,7 @@
 #define DIN6_CROFF DIN6_BIT
 #define DIN6_CR CRL
 #else
-#define DIN6_CROFF (DIN6_BIT&amp;0x03)
+#define DIN6_CROFF (DIN6_BIT&amp;0x05)
 #define DIN6_CR CRH
 #endif
 #define DIO90 90
@@ -8303,7 +8303,7 @@
 #define DIN7_CROFF DIN7_BIT
 #define DIN7_CR CRL
 #else
-#define DIN7_CROFF (DIN7_BIT&amp;0x03)
+#define DIN7_CROFF (DIN7_BIT&amp;0x05)
 #define DIN7_CR CRH
 #endif
 #define DIO91 91
@@ -8371,7 +8371,7 @@
 #define DIN8_CROFF DIN8_BIT
 #define DIN8_CR CRL
 #else
-#define DIN8_CROFF (DIN8_BIT&amp;0x03)
+#define DIN8_CROFF (DIN8_BIT&amp;0x05)
 #define DIN8_CR CRH
 #endif
 #define DIO92 92
@@ -8439,7 +8439,7 @@
 #define DIN9_CROFF DIN9_BIT
 #define DIN9_CR CRL
 #else
-#define DIN9_CROFF (DIN9_BIT&amp;0x03)
+#define DIN9_CROFF (DIN9_BIT&amp;0x05)
 #define DIN9_CR CRH
 #endif
 #define DIO93 93
@@ -8507,7 +8507,7 @@
 #define DIN10_CROFF DIN10_BIT
 #define DIN10_CR CRL
 #else
-#define DIN10_CROFF (DIN10_BIT&amp;0x03)
+#define DIN10_CROFF (DIN10_BIT&amp;0x05)
 #define DIN10_CR CRH
 #endif
 #define DIO94 94
@@ -8575,7 +8575,7 @@
 #define DIN11_CROFF DIN11_BIT
 #define DIN11_CR CRL
 #else
-#define DIN11_CROFF (DIN11_BIT&amp;0x03)
+#define DIN11_CROFF (DIN11_BIT&amp;0x05)
 #define DIN11_CR CRH
 #endif
 #define DIO95 95
@@ -8643,7 +8643,7 @@
 #define DIN12_CROFF DIN12_BIT
 #define DIN12_CR CRL
 #else
-#define DIN12_CROFF (DIN12_BIT&amp;0x03)
+#define DIN12_CROFF (DIN12_BIT&amp;0x05)
 #define DIN12_CR CRH
 #endif
 #define DIO96 96
@@ -8711,7 +8711,7 @@
 #define DIN13_CROFF DIN13_BIT
 #define DIN13_CR CRL
 #else
-#define DIN13_CROFF (DIN13_BIT&amp;0x03)
+#define DIN13_CROFF (DIN13_BIT&amp;0x05)
 #define DIN13_CR CRH
 #endif
 #define DIO97 97
@@ -8779,7 +8779,7 @@
 #define DIN14_CROFF DIN14_BIT
 #define DIN14_CR CRL
 #else
-#define DIN14_CROFF (DIN14_BIT&amp;0x03)
+#define DIN14_CROFF (DIN14_BIT&amp;0x05)
 #define DIN14_CR CRH
 #endif
 #define DIO98 98
@@ -8847,7 +8847,7 @@
 #define DIN15_CROFF DIN15_BIT
 #define DIN15_CR CRL
 #else
-#define DIN15_CROFF (DIN15_BIT&amp;0x03)
+#define DIN15_CROFF (DIN15_BIT&amp;0x05)
 #define DIN15_CR CRH
 #endif
 #define DIO99 99

</xml_diff>